<commit_message>
Added test cases in Dashboard and PIM module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4041E089-2F1C-417E-8D3D-D91FB02E1BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEC7F72B-F808-4057-8A50-566B714567DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Admin" sheetId="3" r:id="rId2"/>
-    <sheet name="PIM" sheetId="4" r:id="rId3"/>
+    <sheet name="Dashboard" sheetId="5" r:id="rId3"/>
+    <sheet name="PIM" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>Admin</t>
   </si>
@@ -90,6 +91,87 @@
   </si>
   <si>
     <t>Peter Anderson</t>
+  </si>
+  <si>
+    <t>TC01_Dashboard_verifyDasboardMainMenus</t>
+  </si>
+  <si>
+    <t>TabName1</t>
+  </si>
+  <si>
+    <t>TabName2</t>
+  </si>
+  <si>
+    <t>TabName3</t>
+  </si>
+  <si>
+    <t>TabName4</t>
+  </si>
+  <si>
+    <t>TabName5</t>
+  </si>
+  <si>
+    <t>TabName6</t>
+  </si>
+  <si>
+    <t>TabName7</t>
+  </si>
+  <si>
+    <t>TabName8</t>
+  </si>
+  <si>
+    <t>TabName9</t>
+  </si>
+  <si>
+    <t>TabName10</t>
+  </si>
+  <si>
+    <t>TabName11</t>
+  </si>
+  <si>
+    <t>PIM</t>
+  </si>
+  <si>
+    <t>Leave</t>
+  </si>
+  <si>
+    <t>Recruitment</t>
+  </si>
+  <si>
+    <t>My Info</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Directory</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Claim</t>
+  </si>
+  <si>
+    <t>Buzz</t>
+  </si>
+  <si>
+    <t>TabName12</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>TC03_PIM_CreateEmployeeWithLoginDetails</t>
+  </si>
+  <si>
+    <t>NewEmployeePassword</t>
+  </si>
+  <si>
+    <t>R29vZHdpbGwxMjM0NQ==</t>
   </si>
 </sst>
 </file>
@@ -569,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F404197-239B-4645-8DB3-C61BAC525CA3}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -624,11 +706,112 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F8DCD4-6953-41BF-9E81-9FEB7A13B9BD}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C437F15-0FF5-4A2F-BDC9-9D3FA98AAE3C}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F8DCD4-6953-41BF-9E81-9FEB7A13B9BD}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -639,7 +822,7 @@
     <col min="4" max="4" width="44.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -647,7 +830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -655,7 +838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -664,12 +847,34 @@
       </c>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added testcases in PIM class
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEC7F72B-F808-4057-8A50-566B714567DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2C4810-9868-4AD1-BF2C-FB0A1B1F593E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>Admin</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>R29vZHdpbGwxMjM0NQ==</t>
+  </si>
+  <si>
+    <t>TC04_PIM_DeleteEmployee</t>
+  </si>
+  <si>
+    <t>TC05_PIM_EditEmployeeName</t>
+  </si>
+  <si>
+    <t>EmployeeNewLastName</t>
+  </si>
+  <si>
+    <t>Sharma</t>
   </si>
 </sst>
 </file>
@@ -257,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -268,6 +280,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F404197-239B-4645-8DB3-C61BAC525CA3}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -808,51 +821,51 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F8DCD4-6953-41BF-9E81-9FEB7A13B9BD}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="44.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
+    <col min="3" max="3" width="56.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -875,6 +888,45 @@
       </c>
       <c r="D6" s="4" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test case in Admin module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2C4810-9868-4AD1-BF2C-FB0A1B1F593E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197D709C-7677-45C4-A44D-EC8C46C84F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>Admin</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Admin1</t>
   </si>
   <si>
-    <t>TC01_Admin_SearchUser</t>
-  </si>
-  <si>
     <t>TC01_Login_ValidCredentials</t>
   </si>
   <si>
@@ -184,6 +181,33 @@
   </si>
   <si>
     <t>Sharma</t>
+  </si>
+  <si>
+    <t>TC01_Admin_SearchUserByNameAndRole</t>
+  </si>
+  <si>
+    <t>TC02_Admin_CreateSystemUser</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>UserPassword</t>
+  </si>
+  <si>
+    <t>EmployeeFirstName</t>
+  </si>
+  <si>
+    <t>EmployeeMiddleName</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>Raj</t>
   </si>
 </sst>
 </file>
@@ -269,10 +293,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -280,7 +303,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,13 +604,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -597,23 +619,23 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -622,7 +644,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -633,7 +655,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -644,13 +666,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>11</v>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -662,10 +684,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F404197-239B-4645-8DB3-C61BAC525CA3}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -676,42 +698,85 @@
     <col min="4" max="4" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
+      <c r="E1" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" s="2"/>
+      <c r="E2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -732,85 +797,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>36</v>
       </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>38</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>39</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>40</v>
       </c>
-      <c r="M2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>21</v>
+      <c r="N2" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -824,7 +889,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -836,97 +901,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="9"/>
+      <c r="A1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>15</v>
+      <c r="B3" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="9"/>
+      <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="B9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>49</v>
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 2 test cases in Admin module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197D709C-7677-45C4-A44D-EC8C46C84F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F2A29A-4052-45F1-B127-A711A9C0CB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
   <si>
     <t>Admin</t>
   </si>
@@ -208,13 +208,34 @@
   </si>
   <si>
     <t>Raj</t>
+  </si>
+  <si>
+    <t>Nidhi</t>
+  </si>
+  <si>
+    <t>TC03_Admin_LoginWithNewSystemUser</t>
+  </si>
+  <si>
+    <t>TC04_Admin_CreateJobTitle</t>
+  </si>
+  <si>
+    <t>JobTitle</t>
+  </si>
+  <si>
+    <t>AssociateQA</t>
+  </si>
+  <si>
+    <t>JobDescription</t>
+  </si>
+  <si>
+    <t>Software Testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +274,23 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -293,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -303,6 +341,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,17 +726,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F404197-239B-4645-8DB3-C61BAC525CA3}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.90625" customWidth="1"/>
     <col min="2" max="2" width="20.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="3" max="3" width="25.36328125" customWidth="1"/>
     <col min="4" max="4" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -776,6 +818,76 @@
       </c>
       <c r="H4" s="3" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 4 test cases in Admin module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5DF21E-5080-479A-99DC-5E6F9FEFF34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151E4F05-F8B3-4308-97E7-9D4F41BA088D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
   <si>
     <t>Admin</t>
   </si>
@@ -229,6 +229,72 @@
   </si>
   <si>
     <t>Software Testing</t>
+  </si>
+  <si>
+    <t>TC05_Admin_CreateEmploymentStatus</t>
+  </si>
+  <si>
+    <t>EmploymentStatus</t>
+  </si>
+  <si>
+    <t>Full-Time Internship</t>
+  </si>
+  <si>
+    <t>JobCategory</t>
+  </si>
+  <si>
+    <t>Search And Online Marketing</t>
+  </si>
+  <si>
+    <t>TC06_Admin_CreateJobCategory</t>
+  </si>
+  <si>
+    <t>TC07_Admin_CreateWorkShift</t>
+  </si>
+  <si>
+    <t>WorkShiftName</t>
+  </si>
+  <si>
+    <t>Morning Shift</t>
+  </si>
+  <si>
+    <t>FromTime</t>
+  </si>
+  <si>
+    <t>ToTime</t>
+  </si>
+  <si>
+    <t>08:00 AM</t>
+  </si>
+  <si>
+    <t>05:00 PM</t>
+  </si>
+  <si>
+    <t>TC08_Admin_CreatePayGrade</t>
+  </si>
+  <si>
+    <t>PayGrade</t>
+  </si>
+  <si>
+    <t>Grade 10</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>MinSalary</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>MaxSalary</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>EUR - Euro</t>
   </si>
 </sst>
 </file>
@@ -331,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -345,6 +411,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,10 +793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F404197-239B-4645-8DB3-C61BAC525CA3}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -888,6 +955,107 @@
       </c>
       <c r="D8" s="12" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 1 test case in Time Module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -1,34 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151E4F05-F8B3-4308-97E7-9D4F41BA088D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F117CF7A-565E-489F-B034-B4497FAB2310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Admin" sheetId="3" r:id="rId2"/>
-    <sheet name="Dashboard" sheetId="5" r:id="rId3"/>
-    <sheet name="PIM" sheetId="4" r:id="rId4"/>
+    <sheet name="Time" sheetId="6" r:id="rId2"/>
+    <sheet name="Admin" sheetId="3" r:id="rId3"/>
+    <sheet name="Dashboard" sheetId="5" r:id="rId4"/>
+    <sheet name="PIM" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="103">
   <si>
     <t>Admin</t>
   </si>
@@ -295,6 +307,48 @@
   </si>
   <si>
     <t>EUR - Euro</t>
+  </si>
+  <si>
+    <t>TC01_Time_CreateTimesheet</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>MonHours</t>
+  </si>
+  <si>
+    <t>TueHours</t>
+  </si>
+  <si>
+    <t>WedHours</t>
+  </si>
+  <si>
+    <t>ThrsHours</t>
+  </si>
+  <si>
+    <t>FriHours</t>
+  </si>
+  <si>
+    <t>TimesheetStatus</t>
+  </si>
+  <si>
+    <t>Krish</t>
+  </si>
+  <si>
+    <t>Apache Software Foundation</t>
+  </si>
+  <si>
+    <t>Bug Fixes</t>
+  </si>
+  <si>
+    <t>8:00</t>
+  </si>
+  <si>
+    <t>Not Submitted</t>
   </si>
 </sst>
 </file>
@@ -397,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -412,6 +466,8 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,19 +753,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.6328125" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" customWidth="1"/>
     <col min="3" max="3" width="20.453125" customWidth="1"/>
     <col min="4" max="4" width="19.81640625" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -784,6 +840,8 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -792,11 +850,104 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30561E53-051B-4245-98F8-1D9446B9D8C0}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F404197-239B-4645-8DB3-C61BAC525CA3}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1063,12 +1214,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C437F15-0FF5-4A2F-BDC9-9D3FA98AAE3C}">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B2" sqref="B2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1164,12 +1315,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F8DCD4-6953-41BF-9E81-9FEB7A13B9BD}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added 2 test cases in Time Module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F117CF7A-565E-489F-B034-B4497FAB2310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD82B0F-5626-4070-901D-D3F5E4FE6C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="121">
   <si>
     <t>Admin</t>
   </si>
@@ -349,6 +349,60 @@
   </si>
   <si>
     <t>Not Submitted</t>
+  </si>
+  <si>
+    <t>TC02_Time_CreateTimesheetWithMultipleProjects</t>
+  </si>
+  <si>
+    <t>Project1</t>
+  </si>
+  <si>
+    <t>Project2</t>
+  </si>
+  <si>
+    <t>Activity1</t>
+  </si>
+  <si>
+    <t>Activity2</t>
+  </si>
+  <si>
+    <t>The Coca-Cola Company</t>
+  </si>
+  <si>
+    <t>NumOfRows</t>
+  </si>
+  <si>
+    <t>Diya</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>TC03_Time_SubmitAndApproveTimesheet</t>
+  </si>
+  <si>
+    <t>Riya</t>
+  </si>
+  <si>
+    <t>TimesheetStatus1</t>
+  </si>
+  <si>
+    <t>TimesheetStatus2</t>
+  </si>
+  <si>
+    <t>TimesheetStatus3</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>ApprovalComment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good.Approved </t>
   </si>
 </sst>
 </file>
@@ -851,15 +905,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30561E53-051B-4245-98F8-1D9446B9D8C0}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>89</v>
       </c>
@@ -873,32 +927,35 @@
         <v>14</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="10"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="10"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="10" t="s">
         <v>58</v>
@@ -909,14 +966,14 @@
       <c r="D2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>101</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>101</v>
@@ -930,14 +987,215 @@
       <c r="K2" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>89</v>
       </c>
     </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="P6" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -947,7 +1205,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added testcase in Recruitment module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD82B0F-5626-4070-901D-D3F5E4FE6C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E983D44F-806C-4043-B05F-6AC18570F9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Time" sheetId="6" r:id="rId2"/>
     <sheet name="Admin" sheetId="3" r:id="rId3"/>
-    <sheet name="Dashboard" sheetId="5" r:id="rId4"/>
-    <sheet name="PIM" sheetId="4" r:id="rId5"/>
+    <sheet name="Recruitment" sheetId="7" r:id="rId4"/>
+    <sheet name="Dashboard" sheetId="5" r:id="rId5"/>
+    <sheet name="PIM" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="132">
   <si>
     <t>Admin</t>
   </si>
@@ -403,6 +404,39 @@
   </si>
   <si>
     <t xml:space="preserve">Good.Approved </t>
+  </si>
+  <si>
+    <t>VacancyName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>QA Automation</t>
+  </si>
+  <si>
+    <t>QA Engineer</t>
+  </si>
+  <si>
+    <t>Collaborate closely with developers, product managers, and other members of the QA team to design and implement robust automation frameworks and test suites.</t>
+  </si>
+  <si>
+    <t>NumOfPositions</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Shah</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>TC01_Recruitment_AddVacancy</t>
+  </si>
+  <si>
+    <t>VacancyStatus</t>
   </si>
 </sst>
 </file>
@@ -505,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -522,6 +556,9 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1204,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F404197-239B-4645-8DB3-C61BAC525CA3}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1473,6 +1510,105 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852351C8-0142-4E1A-A7F3-6BE26A620946}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C437F15-0FF5-4A2F-BDC9-9D3FA98AAE3C}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -1573,7 +1709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F8DCD4-6953-41BF-9E81-9FEB7A13B9BD}">
   <dimension ref="A1:D10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added 2 test cases in Recruitment module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E983D44F-806C-4043-B05F-6AC18570F9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C1A9FD-C549-4843-8172-B1D8079536FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="143">
   <si>
     <t>Admin</t>
   </si>
@@ -97,12 +97,6 @@
     <t>TC01_PIM_CreateEmployeeWithoutCreatingLoginDetails</t>
   </si>
   <si>
-    <t>Peter.Anderson</t>
-  </si>
-  <si>
-    <t>Peter Anderson</t>
-  </si>
-  <si>
     <t>TC01_Dashboard_verifyDasboardMainMenus</t>
   </si>
   <si>
@@ -437,6 +431,45 @@
   </si>
   <si>
     <t>VacancyStatus</t>
+  </si>
+  <si>
+    <t>TC02_Recruitment_AddCandidate</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>CandidateStatus</t>
+  </si>
+  <si>
+    <t>Application Initiated</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>Selenium,JAVA,SQL,Eclipse</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Skilled QA Engineer</t>
+  </si>
+  <si>
+    <t>TC03_Recruitment_ShortlistCandidate</t>
+  </si>
+  <si>
+    <t>Shortlisted</t>
+  </si>
+  <si>
+    <t>CandidateCurrentStatus</t>
+  </si>
+  <si>
+    <t>CandidateInitialStatus</t>
+  </si>
+  <si>
+    <t>Nikhil webTester</t>
   </si>
 </sst>
 </file>
@@ -539,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -556,8 +589,6 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -952,53 +983,53 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="N1" s="10"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>15</v>
@@ -1007,186 +1038,186 @@
         <v>3</v>
       </c>
       <c r="F2" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="I2" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>102</v>
-      </c>
       <c r="N2" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>107</v>
-      </c>
       <c r="J3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="N3" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="O3" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="P3" s="10"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F4" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J4" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" s="10" t="s">
+      <c r="K4" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="O4" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J4" s="15" t="s">
+      <c r="P4" s="12" t="s">
         <v>101</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F5" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="L5" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="K5" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>96</v>
-      </c>
       <c r="M5" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="O5" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="N5" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>116</v>
-      </c>
       <c r="P5" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>15</v>
@@ -1195,40 +1226,40 @@
         <v>3</v>
       </c>
       <c r="F6" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="I6" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="M6" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>102</v>
-      </c>
       <c r="N6" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="O6" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="P6" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="P6" s="10" t="s">
-        <v>120</v>
-      </c>
       <c r="Q6" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1241,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F404197-239B-4645-8DB3-C61BAC525CA3}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1255,7 +1286,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>2</v>
@@ -1275,27 +1306,27 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>14</v>
@@ -1304,44 +1335,44 @@
         <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
@@ -1350,65 +1381,65 @@
         <v>1</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>65</v>
       </c>
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="B8" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="D8" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="1"/>
@@ -1416,92 +1447,92 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
       <c r="B10" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
       <c r="B12" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>76</v>
-      </c>
       <c r="D13" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
       <c r="B14" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>83</v>
-      </c>
       <c r="D15" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="10"/>
       <c r="B16" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="F16" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1511,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852351C8-0142-4E1A-A7F3-6BE26A620946}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1529,13 +1560,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>14</v>
@@ -1544,63 +1575,173 @@
         <v>1</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>131</v>
+      <c r="H1" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="L2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="C3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" t="s">
+        <v>137</v>
+      </c>
+      <c r="H4" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" t="s">
+        <v>133</v>
+      </c>
+      <c r="I6" t="s">
+        <v>139</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1623,43 +1764,43 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="M1" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -1667,40 +1808,40 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>35</v>
       </c>
-      <c r="H2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>36</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>38</v>
       </c>
-      <c r="L2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" t="s">
-        <v>40</v>
-      </c>
       <c r="N2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1760,13 +1901,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1774,15 +1915,15 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>14</v>
@@ -1794,18 +1935,18 @@
         <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -1813,10 +1954,10 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 3 test cases in Recruitment module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C1A9FD-C549-4843-8172-B1D8079536FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCCFF99-0091-4852-BC01-41D08EFCC2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="157">
   <si>
     <t>Admin</t>
   </si>
@@ -470,6 +470,48 @@
   </si>
   <si>
     <t>Nikhil webTester</t>
+  </si>
+  <si>
+    <t>Interview Scheduled</t>
+  </si>
+  <si>
+    <t>DateOfInterview</t>
+  </si>
+  <si>
+    <t>TimeOfInterview</t>
+  </si>
+  <si>
+    <t>02:00 PM</t>
+  </si>
+  <si>
+    <t>InterviewTitle</t>
+  </si>
+  <si>
+    <t>Automation Tester</t>
+  </si>
+  <si>
+    <t>TC04_Recruitment_ScheduleInterviewForCandidate</t>
+  </si>
+  <si>
+    <t>2024-18-03</t>
+  </si>
+  <si>
+    <t>TC05_Recruitment_MarkInterviewPassedAndOfferJobToCandidate</t>
+  </si>
+  <si>
+    <t>CandidateStatus2</t>
+  </si>
+  <si>
+    <t>Interview Passed</t>
+  </si>
+  <si>
+    <t>Job Offered</t>
+  </si>
+  <si>
+    <t>Hired</t>
+  </si>
+  <si>
+    <t>TC06_Recruitment_HireCandidate</t>
   </si>
 </sst>
 </file>
@@ -572,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -590,6 +632,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1272,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F404197-239B-4645-8DB3-C61BAC525CA3}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1542,10 +1585,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{852351C8-0142-4E1A-A7F3-6BE26A620946}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1554,7 +1597,7 @@
     <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.90625" customWidth="1"/>
     <col min="7" max="7" width="23.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1742,6 +1785,168 @@
       </c>
       <c r="J6" s="3" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I8" t="s">
+        <v>139</v>
+      </c>
+      <c r="J8" t="s">
+        <v>143</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G10" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" t="s">
+        <v>154</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G12" t="s">
+        <v>155</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 1 test case in Dashboard
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SharikaNarayananNamb\git\Framework\SeleniumFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FF3AAC-BA22-45D1-95A0-DD0DBABB0761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E79E7694-1F5C-4B19-93F0-52DCB46700A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="178">
   <si>
     <t>Admin</t>
   </si>
@@ -572,6 +572,9 @@
   </si>
   <si>
     <t>Fun Shift</t>
+  </si>
+  <si>
+    <t>TC02_Dashboard_PunchInAndPunchOutFromDasboard</t>
   </si>
 </sst>
 </file>
@@ -1375,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F404197-239B-4645-8DB3-C61BAC525CA3}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1648,7 +1651,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2180,10 +2183,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C437F15-0FF5-4A2F-BDC9-9D3FA98AAE3C}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2271,6 +2274,28 @@
       </c>
       <c r="N2" s="3" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2284,7 +2309,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A5" sqref="A5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>